<commit_message>
add configures for journal, kdump, ...
</commit_message>
<xml_diff>
--- a/hardening-description.xlsx
+++ b/hardening-description.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="210">
   <si>
     <t>PASS_MAX_DAYS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -588,16 +588,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>touch /var/log/sudo.log
-chmod 400 /var/log/sudo.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/etc/sudoers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Defaults logfile=/var/log/sudo.log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -872,6 +863,60 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>close</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sftp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UseDNS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/etc/ntp.conf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/etc/sysconfig/ntpd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/etc/ntp/step-tickers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/etc/sysconfig/ntpdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>追加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127.0.0.1 {{fqdn}} {{hostname}}
+::1 {{fqdn}} {{hostname}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>touch /var/log/sudo.log
+chmod 400 /var/log/sudo.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defaults logfile=/var/log/sudo.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sudo.log转储</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>/etc/security/opasswd.old
 /var/log/dmesg/dmesg.old
 /etc/udev/rules.d/*
@@ -880,56 +925,12 @@
 /etc/yum.repos.d/*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>sftp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>close</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/etc/ssh/sshd_config</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sftp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UseDNS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/etc/ntp.conf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/etc/sysconfig/ntpd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/etc/ntp/step-tickers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/etc/sysconfig/ntpdate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>追加</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1003,6 +1004,15 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1073,12 +1083,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1151,13 +1161,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1365,9 +1387,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1377,42 +1396,171 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1425,36 +1573,25 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1744,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1786,10 +1923,10 @@
       <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89">
+      <c r="A2" s="110">
         <v>1</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="111" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -1807,11 +1944,11 @@
       <c r="G2" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="79"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="90"/>
+      <c r="A3" s="110"/>
+      <c r="B3" s="111"/>
       <c r="C3" s="9" t="s">
         <v>48</v>
       </c>
@@ -1825,13 +1962,13 @@
       <c r="G3" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="79"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92">
+      <c r="A4" s="117">
         <v>2</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="114" t="s">
         <v>94</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -1843,17 +1980,17 @@
       <c r="E4" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="69" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="78"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
-      <c r="B5" s="91"/>
+      <c r="A5" s="118"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="12" t="s">
         <v>97</v>
       </c>
@@ -1863,57 +2000,57 @@
       <c r="E5" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="70" t="s">
+      <c r="F5" s="69" t="s">
         <v>105</v>
       </c>
       <c r="G5" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="H5" s="78"/>
+      <c r="H5" s="73"/>
     </row>
     <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="118"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="12" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E6" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="F6" s="69" t="s">
         <v>105</v>
       </c>
       <c r="G6" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="78"/>
+      <c r="H6" s="73"/>
     </row>
     <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="119"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="12" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E7" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="70" t="s">
+      <c r="F7" s="69" t="s">
         <v>105</v>
       </c>
       <c r="G7" s="57"/>
-      <c r="H7" s="78"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="94">
+      <c r="A8" s="113">
         <v>3</v>
       </c>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="112" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="58" t="s">
@@ -1925,17 +2062,17 @@
       <c r="E8" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="70" t="s">
+      <c r="F8" s="69" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="H8" s="78"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
-      <c r="B9" s="93"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="58" t="s">
         <v>4</v>
       </c>
@@ -1945,13 +2082,13 @@
       <c r="E9" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="70" t="s">
+      <c r="F9" s="69" t="s">
         <v>106</v>
       </c>
       <c r="G9" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="H9" s="78"/>
+      <c r="H9" s="73"/>
     </row>
     <row r="10" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
@@ -1975,7 +2112,7 @@
       <c r="G10" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="H10" s="78"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
@@ -1987,17 +2124,19 @@
       <c r="C11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="77" t="s">
         <v>109</v>
       </c>
       <c r="E11" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="70" t="s">
+      <c r="F11" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="76"/>
+      <c r="G11" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="73"/>
     </row>
     <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32">
@@ -2012,18 +2151,18 @@
       <c r="D12" s="34"/>
       <c r="E12" s="8"/>
       <c r="F12" s="65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G12" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="76"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="86">
+      <c r="A13" s="107">
         <v>7</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="104" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -2031,67 +2170,67 @@
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="55" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>112</v>
       </c>
       <c r="G13" s="24"/>
-      <c r="H13" s="78"/>
+      <c r="H13" s="73"/>
     </row>
     <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="87"/>
-      <c r="B14" s="85"/>
+      <c r="A14" s="108"/>
+      <c r="B14" s="105"/>
       <c r="C14" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F14" s="27" t="s">
         <v>112</v>
       </c>
       <c r="G14" s="24"/>
-      <c r="H14" s="78"/>
+      <c r="H14" s="73"/>
     </row>
     <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="87"/>
-      <c r="B15" s="85"/>
+      <c r="A15" s="108"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="11" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F15" s="27" t="s">
         <v>112</v>
       </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="78"/>
+      <c r="H15" s="73"/>
     </row>
     <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="F16" s="70" t="s">
+      <c r="A16" s="108"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="81" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="82" t="s">
+        <v>202</v>
+      </c>
+      <c r="F16" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="76"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="79"/>
     </row>
     <row r="17" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
-      <c r="B17" s="85"/>
+      <c r="A17" s="108"/>
+      <c r="B17" s="105"/>
       <c r="C17" s="29" t="s">
         <v>37</v>
       </c>
@@ -2105,25 +2244,25 @@
         <v>90</v>
       </c>
       <c r="G17" s="24"/>
-      <c r="H17" s="78"/>
+      <c r="H17" s="73"/>
     </row>
     <row r="18" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
-      <c r="B18" s="84"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="106"/>
       <c r="C18" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G18" s="24"/>
-      <c r="H18" s="78"/>
+      <c r="H18" s="73"/>
     </row>
     <row r="19" spans="1:8" ht="85.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="51">
@@ -2145,7 +2284,7 @@
       <c r="G19" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="H19" s="80"/>
+      <c r="H19" s="75"/>
     </row>
     <row r="20" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32">
@@ -2162,12 +2301,12 @@
       </c>
       <c r="E20" s="33"/>
       <c r="F20" s="65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G20" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="H20" s="76"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
@@ -2177,7 +2316,7 @@
         <v>127</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="11" t="s">
@@ -2187,9 +2326,9 @@
         <v>112</v>
       </c>
       <c r="G21" s="24"/>
-      <c r="H21" s="97"/>
-    </row>
-    <row r="22" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="73"/>
+    </row>
+    <row r="22" spans="1:8" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>11</v>
       </c>
@@ -2197,269 +2336,276 @@
         <v>128</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D22" s="10"/>
+        <v>137</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>205</v>
+      </c>
       <c r="E22" s="11" t="s">
         <v>123</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G22" s="24"/>
-      <c r="H22" s="77"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
+      <c r="A23" s="80">
         <v>12</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="41" t="s">
+      <c r="D23" s="84"/>
+      <c r="E23" s="85" t="s">
         <v>124</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="H23" s="76"/>
+      <c r="H23" s="79"/>
     </row>
     <row r="24" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="81">
+      <c r="A24" s="120">
         <v>13</v>
       </c>
-      <c r="B24" s="83" t="s">
-        <v>133</v>
+      <c r="B24" s="104" t="s">
+        <v>131</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="41" t="s">
-        <v>130</v>
+        <v>206</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="76"/>
+      <c r="H24" s="73"/>
     </row>
     <row r="25" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="82"/>
-      <c r="B25" s="84"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>132</v>
+        <v>207</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="69" t="s">
         <v>105</v>
       </c>
       <c r="G25" s="16"/>
-      <c r="H25" s="76"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="74"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="76"/>
+      <c r="A26" s="122"/>
+      <c r="B26" s="106"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="86" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
         <v>14</v>
       </c>
       <c r="B27" s="55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F27" s="27" t="s">
         <v>77</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="76"/>
+      <c r="H27" s="73"/>
     </row>
     <row r="28" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="81">
+      <c r="A28" s="125">
         <v>15</v>
       </c>
-      <c r="B28" s="83" t="s">
-        <v>145</v>
+      <c r="B28" s="123" t="s">
+        <v>143</v>
       </c>
       <c r="C28" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="73"/>
+    </row>
+    <row r="29" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="126"/>
+      <c r="B29" s="124"/>
+      <c r="C29" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="F28" s="70" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="16"/>
-      <c r="H28" s="78"/>
-    </row>
-    <row r="29" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="82"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>98</v>
       </c>
       <c r="E29" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="73"/>
+    </row>
+    <row r="30" spans="1:8" s="70" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="110">
+        <v>16</v>
+      </c>
+      <c r="B30" s="111" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="F29" s="70" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="78"/>
-    </row>
-    <row r="30" spans="1:8" s="71" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="89">
-        <v>16</v>
-      </c>
-      <c r="B30" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="C30" s="29" t="s">
+      <c r="D30" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="31" t="s">
         <v>146</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="E30" s="31" t="s">
-        <v>148</v>
       </c>
       <c r="F30" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G30" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="H30" s="73"/>
+    </row>
+    <row r="31" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="110"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="31" t="s">
         <v>149</v>
-      </c>
-      <c r="H30" s="97"/>
-    </row>
-    <row r="31" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="89"/>
-      <c r="B31" s="90"/>
-      <c r="C31" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>151</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G31" s="16"/>
-      <c r="H31" s="97"/>
+      <c r="H31" s="73"/>
     </row>
     <row r="32" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="89">
+      <c r="A32" s="110">
         <v>17</v>
       </c>
-      <c r="B32" s="90" t="s">
-        <v>155</v>
+      <c r="B32" s="111" t="s">
+        <v>153</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G32" s="16"/>
-      <c r="H32" s="76"/>
+      <c r="H32" s="73"/>
     </row>
     <row r="33" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="89"/>
-      <c r="B33" s="90"/>
+      <c r="A33" s="110"/>
+      <c r="B33" s="111"/>
       <c r="C33" s="29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G33" s="16"/>
-      <c r="H33" s="97"/>
+      <c r="H33" s="73"/>
     </row>
     <row r="34" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="89"/>
-      <c r="B34" s="90"/>
+      <c r="A34" s="110"/>
+      <c r="B34" s="111"/>
       <c r="C34" s="29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F34" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G34" s="16"/>
-      <c r="H34" s="97"/>
+      <c r="H34" s="73"/>
     </row>
     <row r="35" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="89"/>
-      <c r="B35" s="90"/>
+      <c r="A35" s="110"/>
+      <c r="B35" s="111"/>
       <c r="C35" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F35" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" s="69" t="s">
         <v>27</v>
       </c>
       <c r="G35" s="16"/>
+      <c r="H35" s="73"/>
     </row>
     <row r="36" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>18</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C36" s="29" t="s">
         <v>69</v>
@@ -2474,74 +2620,74 @@
         <v>90</v>
       </c>
       <c r="G36" s="16"/>
-      <c r="H36" s="97"/>
+      <c r="H36" s="73"/>
     </row>
     <row r="37" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
         <v>19</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F37" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G37" s="16"/>
-      <c r="H37" s="97"/>
+      <c r="H37" s="73"/>
     </row>
     <row r="38" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29">
+      <c r="A38" s="80">
         <v>20</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
+      <c r="B38" s="82" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="83"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="82"/>
       <c r="F38" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G38" s="16"/>
-      <c r="H38" s="76"/>
+        <v>83</v>
+      </c>
+      <c r="G38" s="86"/>
+      <c r="H38" s="79"/>
     </row>
     <row r="39" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
         <v>21</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D39" s="30" t="s">
         <v>42</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F39" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G39" s="16"/>
-      <c r="H39" s="97"/>
+      <c r="H39" s="73"/>
     </row>
     <row r="40" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
         <v>22</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C40" s="29" t="s">
         <v>41</v>
@@ -2556,14 +2702,14 @@
         <v>90</v>
       </c>
       <c r="G40" s="16"/>
-      <c r="H40" s="97"/>
+      <c r="H40" s="73"/>
     </row>
     <row r="41" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
         <v>23</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C41" s="29" t="s">
         <v>64</v>
@@ -2578,234 +2724,231 @@
         <v>90</v>
       </c>
       <c r="G41" s="16"/>
-      <c r="H41" s="97"/>
+      <c r="H41" s="73"/>
     </row>
     <row r="42" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="86">
+      <c r="A42" s="128">
         <v>24</v>
       </c>
-      <c r="B42" s="83" t="s">
-        <v>179</v>
+      <c r="B42" s="123" t="s">
+        <v>177</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D42" s="30"/>
-      <c r="E42" s="72" t="s">
-        <v>180</v>
+      <c r="E42" s="71" t="s">
+        <v>178</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G42" s="16"/>
-      <c r="H42" s="80"/>
+      <c r="H42" s="75"/>
     </row>
     <row r="43" spans="1:8" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="87"/>
-      <c r="B43" s="85"/>
+      <c r="A43" s="129"/>
+      <c r="B43" s="127"/>
       <c r="C43" s="29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D43" s="30"/>
-      <c r="E43" s="72" t="s">
-        <v>181</v>
+      <c r="E43" s="71" t="s">
+        <v>179</v>
       </c>
       <c r="F43" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G43" s="16"/>
-      <c r="H43" s="80"/>
+      <c r="H43" s="75"/>
     </row>
     <row r="44" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="88"/>
-      <c r="B44" s="84"/>
+      <c r="A44" s="130"/>
+      <c r="B44" s="124"/>
       <c r="C44" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="41" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F44" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G44" s="16"/>
-      <c r="H44" s="80"/>
+      <c r="H44" s="75"/>
     </row>
     <row r="45" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29">
+      <c r="A45" s="80">
         <v>25</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="10" t="s">
+      <c r="B45" s="82" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="83"/>
+      <c r="D45" s="84" t="s">
+        <v>185</v>
+      </c>
+      <c r="E45" s="82" t="s">
+        <v>184</v>
+      </c>
+      <c r="F45" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="86"/>
+      <c r="H45" s="79"/>
+    </row>
+    <row r="46" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="128">
+        <v>26</v>
+      </c>
+      <c r="B46" s="123" t="s">
         <v>187</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F45" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="G45" s="16"/>
-      <c r="H45" s="76"/>
-    </row>
-    <row r="46" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="86">
-        <v>26</v>
-      </c>
-      <c r="B46" s="83" t="s">
-        <v>189</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="10"/>
       <c r="E46" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F46" s="70" t="s">
+        <v>188</v>
+      </c>
+      <c r="F46" s="69" t="s">
         <v>27</v>
       </c>
       <c r="G46" s="16"/>
-      <c r="H46" s="76"/>
+      <c r="H46" s="73"/>
     </row>
     <row r="47" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="88"/>
-      <c r="B47" s="84"/>
+      <c r="A47" s="130"/>
+      <c r="B47" s="124"/>
       <c r="C47" s="11"/>
       <c r="D47" s="10"/>
       <c r="E47" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="16"/>
+      <c r="H47" s="73"/>
+    </row>
+    <row r="48" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="80">
+        <v>27</v>
+      </c>
+      <c r="B48" s="82" t="s">
         <v>191</v>
       </c>
-      <c r="F47" s="70" t="s">
+      <c r="C48" s="82"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="82" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="G47" s="16"/>
-      <c r="H47" s="76"/>
-    </row>
-    <row r="48" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="29">
+      <c r="G48" s="86"/>
+      <c r="H48" s="79"/>
+    </row>
+    <row r="49" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="80">
+        <v>28</v>
+      </c>
+      <c r="B49" s="82" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="82"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="G49" s="86"/>
+      <c r="H49" s="79"/>
+    </row>
+    <row r="50" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="107">
+        <v>29</v>
+      </c>
+      <c r="B50" s="104" t="s">
         <v>193</v>
-      </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="F48" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="G48" s="16"/>
-      <c r="H48" s="76"/>
-    </row>
-    <row r="49" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="29">
-        <v>28</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="G49" s="16"/>
-      <c r="H49" s="76"/>
-    </row>
-    <row r="50" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="86">
-        <v>29</v>
-      </c>
-      <c r="B50" s="83" t="s">
-        <v>195</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="10"/>
       <c r="E50" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="F50" s="70" t="s">
+        <v>194</v>
+      </c>
+      <c r="F50" s="69" t="s">
         <v>27</v>
       </c>
       <c r="G50" s="16"/>
-      <c r="H50" s="76"/>
+      <c r="H50" s="79"/>
     </row>
     <row r="51" spans="1:8" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="87"/>
-      <c r="B51" s="85"/>
+      <c r="A51" s="108"/>
+      <c r="B51" s="105"/>
       <c r="C51" s="11"/>
       <c r="D51" s="10"/>
       <c r="E51" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="F51" s="75" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" s="72" t="s">
         <v>30</v>
       </c>
       <c r="G51" s="16"/>
-      <c r="H51" s="76"/>
+      <c r="H51" s="79"/>
     </row>
     <row r="52" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="88"/>
-      <c r="B52" s="84"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="F52" s="15"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="76"/>
+      <c r="A52" s="108"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="76" t="s">
+        <v>195</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52" s="97"/>
+      <c r="H52" s="135"/>
     </row>
     <row r="53" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="29">
-        <v>30</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="F53" s="15"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="76"/>
+      <c r="A53" s="98"/>
+      <c r="B53" s="99"/>
+      <c r="C53" s="99"/>
+      <c r="D53" s="100"/>
+      <c r="E53" s="99"/>
+      <c r="F53" s="101"/>
+      <c r="G53" s="102"/>
+      <c r="H53" s="103"/>
     </row>
     <row r="54" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
+      <c r="A54" s="91"/>
+      <c r="B54" s="92"/>
+      <c r="C54" s="92"/>
+      <c r="D54" s="93"/>
+      <c r="E54" s="92"/>
+      <c r="F54" s="94"/>
+      <c r="G54" s="94"/>
+      <c r="H54" s="95"/>
     </row>
     <row r="55" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
+      <c r="A55" s="91"/>
+      <c r="B55" s="92"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="92"/>
+      <c r="F55" s="94"/>
+      <c r="G55" s="94"/>
+      <c r="H55" s="95"/>
     </row>
     <row r="56" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
+      <c r="A56" s="87"/>
+      <c r="B56" s="88"/>
+      <c r="C56" s="88"/>
+      <c r="D56" s="89"/>
+      <c r="E56" s="88"/>
+      <c r="F56" s="90"/>
+      <c r="G56" s="90"/>
+      <c r="H56" s="70"/>
     </row>
     <row r="57" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="26"/>
@@ -3500,26 +3643,29 @@
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A4:A7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3527,8 +3673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" activeCellId="2" sqref="C16:E16 C14:E14 C22:E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3568,10 +3714,10 @@
       <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89">
+      <c r="A2" s="110">
         <v>1</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="111" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -3580,7 +3726,7 @@
       <c r="D2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="90" t="s">
+      <c r="E2" s="111" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="15" t="s">
@@ -3589,40 +3735,40 @@
       <c r="G2" s="24"/>
     </row>
     <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="90"/>
+      <c r="A3" s="110"/>
+      <c r="B3" s="111"/>
       <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="90"/>
+      <c r="E3" s="111"/>
       <c r="F3" s="15" t="s">
         <v>27</v>
       </c>
       <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="90"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="111"/>
       <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="90"/>
+      <c r="E4" s="111"/>
       <c r="F4" s="15" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92">
+      <c r="A5" s="131">
         <v>2</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="132" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -3640,8 +3786,8 @@
       <c r="G5" s="49"/>
     </row>
     <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
-      <c r="B6" s="91"/>
+      <c r="A6" s="131"/>
+      <c r="B6" s="132"/>
       <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
@@ -3680,10 +3826,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="92">
+      <c r="A8" s="131">
         <v>4</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="132" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -3692,7 +3838,7 @@
       <c r="D8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="91" t="s">
+      <c r="E8" s="132" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="19" t="s">
@@ -3703,15 +3849,15 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="92"/>
-      <c r="B9" s="91"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="91"/>
+      <c r="E9" s="132"/>
       <c r="F9" s="19" t="s">
         <v>27</v>
       </c>
@@ -3720,40 +3866,40 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="92"/>
-      <c r="B10" s="91"/>
+      <c r="A10" s="131"/>
+      <c r="B10" s="132"/>
       <c r="C10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="91"/>
+      <c r="E10" s="132"/>
       <c r="F10" s="19" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="49"/>
     </row>
     <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
-      <c r="B11" s="91"/>
+      <c r="A11" s="131"/>
+      <c r="B11" s="132"/>
       <c r="C11" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="91"/>
+      <c r="E11" s="132"/>
       <c r="F11" s="19" t="s">
         <v>30</v>
       </c>
       <c r="G11" s="49"/>
     </row>
     <row r="12" spans="1:8" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="89">
+      <c r="A12" s="110">
         <v>5</v>
       </c>
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="111" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -3771,8 +3917,8 @@
       <c r="G12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="89"/>
-      <c r="B13" s="90"/>
+      <c r="A13" s="110"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="9" t="s">
         <v>48</v>
       </c>
@@ -3788,8 +3934,8 @@
       <c r="G13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="89"/>
-      <c r="B14" s="90"/>
+      <c r="A14" s="110"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="29" t="s">
         <v>37</v>
       </c>
@@ -3805,8 +3951,8 @@
       <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="89"/>
-      <c r="B15" s="90"/>
+      <c r="A15" s="110"/>
+      <c r="B15" s="111"/>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
@@ -3822,8 +3968,8 @@
       <c r="G15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="89"/>
-      <c r="B16" s="90"/>
+      <c r="A16" s="110"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="29" t="s">
         <v>41</v>
       </c>
@@ -3839,8 +3985,8 @@
       <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="89"/>
-      <c r="B17" s="90"/>
+      <c r="A17" s="110"/>
+      <c r="B17" s="111"/>
       <c r="C17" s="9" t="s">
         <v>48</v>
       </c>
@@ -3854,8 +4000,8 @@
       <c r="G17" s="24"/>
     </row>
     <row r="18" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
-      <c r="B18" s="90"/>
+      <c r="A18" s="110"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="9" t="s">
         <v>48</v>
       </c>
@@ -3890,10 +4036,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="95">
+      <c r="A20" s="133">
         <v>7</v>
       </c>
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="111" t="s">
         <v>61</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -3909,8 +4055,8 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
-      <c r="B21" s="90"/>
+      <c r="A21" s="133"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="9" t="s">
         <v>48</v>
       </c>
@@ -3924,8 +4070,8 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
-      <c r="B22" s="90"/>
+      <c r="A22" s="133"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="29" t="s">
         <v>64</v>
       </c>
@@ -3941,10 +4087,10 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="96">
+      <c r="A23" s="134">
         <v>8</v>
       </c>
-      <c r="B23" s="91" t="s">
+      <c r="B23" s="132" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="35" t="s">
@@ -3962,8 +4108,8 @@
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="96"/>
-      <c r="B24" s="91"/>
+      <c r="A24" s="134"/>
+      <c r="B24" s="132"/>
       <c r="C24" s="12" t="s">
         <v>73</v>
       </c>
@@ -3999,7 +4145,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" s="71" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="70" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>10</v>
       </c>
@@ -4142,15 +4288,15 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>